<commit_message>
vault backup: 2024-12-03 12:19:06
</commit_message>
<xml_diff>
--- a/FP/공연정보FP.xlsx
+++ b/FP/공연정보FP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이준한\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Greatbps\Pusan\FP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1C9F763-A206-4D25-BB4C-F55C072BE93C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC538AB-C55B-4B43-9547-2B785E0D552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13095" xr2:uid="{1257D84A-1ED9-4987-8E0A-839B2EB2420D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21240" windowHeight="12780" xr2:uid="{1257D84A-1ED9-4987-8E0A-839B2EB2420D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="119">
   <si>
     <t>1. 회원 관리</t>
   </si>
@@ -902,6 +913,26 @@
   </si>
   <si>
     <t>할인 조건 등록</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 예약 및 결제 관리</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 할인/감면 관리</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 이벤트 및 프로모션 관리</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 시설 관리</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 통계 및 선호도 분석</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -1194,7 +1225,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5BB21AC-F308-4370-A1F0-A19B6F623EED}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1225,9 +1256,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1265,7 +1296,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1371,7 +1402,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1513,7 +1544,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1524,8 +1555,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="E1:H309"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1754,7 +1785,7 @@
     </row>
     <row r="35" spans="5:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="E35" s="10" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="5:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1886,7 +1917,7 @@
     </row>
     <row r="53" spans="5:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="E53" s="10" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="5:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1984,7 +2015,7 @@
     </row>
     <row r="69" spans="5:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="E69" s="10" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="5:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2074,7 +2105,7 @@
     </row>
     <row r="84" spans="5:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="E84" s="10" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="5:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2150,7 +2181,7 @@
     </row>
     <row r="98" spans="5:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="E98" s="10" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
     </row>
     <row r="99" spans="5:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2530,7 +2561,7 @@
     <row r="171" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E171" s="1"/>
     </row>
-    <row r="172" spans="5:8" ht="99" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E172" s="2" t="s">
         <v>8</v>
       </c>
@@ -2639,7 +2670,7 @@
     <row r="181" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E181" s="1"/>
     </row>
-    <row r="182" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E182" s="7" t="s">
         <v>21</v>
       </c>
@@ -2662,7 +2693,7 @@
     <row r="189" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E189" s="1"/>
     </row>
-    <row r="190" spans="5:8" ht="99" x14ac:dyDescent="0.3">
+    <row r="190" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E190" s="2" t="s">
         <v>22</v>
       </c>
@@ -2771,7 +2802,7 @@
     <row r="199" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E199" s="1"/>
     </row>
-    <row r="200" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="200" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E200" s="7" t="s">
         <v>35</v>
       </c>
@@ -2794,7 +2825,7 @@
     <row r="207" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E207" s="1"/>
     </row>
-    <row r="208" spans="5:8" ht="99" x14ac:dyDescent="0.3">
+    <row r="208" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E208" s="2" t="s">
         <v>36</v>
       </c>
@@ -2875,7 +2906,7 @@
     <row r="215" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E215" s="1"/>
     </row>
-    <row r="216" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="216" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E216" s="7" t="s">
         <v>45</v>
       </c>
@@ -2898,7 +2929,7 @@
     <row r="223" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E223" s="1"/>
     </row>
-    <row r="224" spans="5:8" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="224" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E224" s="2" t="s">
         <v>46</v>
       </c>
@@ -2965,7 +2996,7 @@
     <row r="230" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E230" s="1"/>
     </row>
-    <row r="231" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="231" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E231" s="7" t="s">
         <v>53</v>
       </c>
@@ -2988,7 +3019,7 @@
     <row r="238" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E238" s="1"/>
     </row>
-    <row r="239" spans="5:8" ht="74.25" x14ac:dyDescent="0.3">
+    <row r="239" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E239" s="2" t="s">
         <v>54</v>
       </c>
@@ -3041,7 +3072,7 @@
     <row r="244" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E244" s="1"/>
     </row>
-    <row r="245" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="245" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E245" s="7" t="s">
         <v>59</v>
       </c>
@@ -3064,7 +3095,7 @@
     <row r="252" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E252" s="1"/>
     </row>
-    <row r="253" spans="5:8" ht="123.75" x14ac:dyDescent="0.3">
+    <row r="253" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E253" s="2" t="s">
         <v>60</v>
       </c>
@@ -3131,7 +3162,7 @@
     <row r="259" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E259" s="1"/>
     </row>
-    <row r="260" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="260" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E260" s="7" t="s">
         <v>67</v>
       </c>
@@ -3154,7 +3185,7 @@
     <row r="267" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E267" s="1"/>
     </row>
-    <row r="268" spans="5:8" ht="99" x14ac:dyDescent="0.3">
+    <row r="268" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E268" s="2" t="s">
         <v>68</v>
       </c>
@@ -3221,7 +3252,7 @@
     <row r="274" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E274" s="1"/>
     </row>
-    <row r="275" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="275" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E275" s="7" t="s">
         <v>75</v>
       </c>
@@ -3244,7 +3275,7 @@
     <row r="282" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E282" s="1"/>
     </row>
-    <row r="283" spans="5:8" ht="74.25" x14ac:dyDescent="0.3">
+    <row r="283" spans="5:8" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E283" s="2" t="s">
         <v>76</v>
       </c>
@@ -3283,7 +3314,7 @@
     <row r="287" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E287" s="1"/>
     </row>
-    <row r="288" spans="5:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="288" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E288" s="7" t="s">
         <v>79</v>
       </c>
@@ -3306,7 +3337,7 @@
     <row r="295" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E295" s="1"/>
     </row>
-    <row r="296" spans="5:6" ht="74.25" x14ac:dyDescent="0.3">
+    <row r="296" spans="5:6" ht="24.75" x14ac:dyDescent="0.3">
       <c r="E296" s="2" t="s">
         <v>80</v>
       </c>
@@ -3330,7 +3361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="5:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="5:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E300" s="9" t="s">
         <v>84</v>
       </c>
@@ -3338,7 +3369,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="301" spans="5:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="5:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E301" s="9" t="s">
         <v>85</v>
       </c>
@@ -3346,7 +3377,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="302" spans="5:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="5:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E302" s="9" t="s">
         <v>86</v>
       </c>
@@ -3354,7 +3385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="303" spans="5:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="5:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E303" s="9" t="s">
         <v>87</v>
       </c>
@@ -3370,7 +3401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="305" spans="5:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="5:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E305" s="9" t="s">
         <v>89</v>
       </c>
@@ -3378,7 +3409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="306" spans="5:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="5:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E306" s="9" t="s">
         <v>90</v>
       </c>
@@ -3386,7 +3417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="307" spans="5:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="5:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E307" s="9" t="s">
         <v>91</v>
       </c>
@@ -3397,7 +3428,7 @@
     <row r="308" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E308" s="1"/>
     </row>
-    <row r="309" spans="5:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="309" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E309" s="7" t="s">
         <v>92</v>
       </c>

</xml_diff>